<commit_message>
created the vehicle dashboard
</commit_message>
<xml_diff>
--- a/public/assets/Page_Layout.xlsx
+++ b/public/assets/Page_Layout.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\Documents\GitHub\auto-tracker\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\Documents\GitHub\auto-tracker\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E76C8CE-4A17-489C-8B7A-79E2227FB862}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03D1105-58DD-4513-9581-6AA8344B9267}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" firstSheet="2" activeTab="6" xr2:uid="{DDC1677D-DCB0-46BC-99F7-D600D37E193E}"/>
   </bookViews>
@@ -241,7 +241,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,6 +275,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -444,14 +474,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1162,11 +1197,11 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
@@ -1190,7 +1225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3E8A2C-78ED-4C05-8353-A07A1699F673}">
   <dimension ref="B2:J24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5:L26"/>
     </sheetView>
   </sheetViews>
@@ -1477,418 +1512,922 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F59211D-0CF4-40FF-9215-F8BE8347E42A}">
-  <dimension ref="C2:Q25"/>
+  <dimension ref="C2:Q101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:O19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
     </row>
     <row r="3" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
     </row>
     <row r="4" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
     </row>
     <row r="8" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
     </row>
     <row r="9" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
     </row>
     <row r="10" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
     </row>
     <row r="11" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
     </row>
     <row r="12" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
     </row>
     <row r="13" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C13" s="19"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
+      <c r="C13" s="18"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
     </row>
     <row r="14" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C14" s="19"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
+      <c r="C14" s="18"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
     </row>
     <row r="15" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
     </row>
     <row r="16" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
     </row>
     <row r="17" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C18" s="19"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
+      <c r="G18" s="18"/>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
       <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
     </row>
     <row r="19" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C19" s="19"/>
+      <c r="C19" s="18"/>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
+      <c r="G19" s="18"/>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="19"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C20" s="19"/>
+      <c r="C20" s="18"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="19"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="20"/>
     </row>
     <row r="21" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C21" s="19"/>
+      <c r="C21" s="18"/>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
+      <c r="G21" s="18"/>
       <c r="H21" s="19"/>
       <c r="I21" s="19"/>
       <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="20"/>
     </row>
     <row r="22" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C22" s="19"/>
+      <c r="C22" s="18"/>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
+      <c r="G22" s="18"/>
       <c r="H22" s="19"/>
       <c r="I22" s="19"/>
       <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="19"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
     </row>
     <row r="23" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C23" s="19"/>
+      <c r="C23" s="18"/>
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
+      <c r="G23" s="18"/>
       <c r="H23" s="19"/>
       <c r="I23" s="19"/>
       <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="19"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
     </row>
     <row r="24" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="19"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
     </row>
     <row r="25" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+    </row>
+    <row r="39" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="20"/>
+    </row>
+    <row r="40" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+    </row>
+    <row r="41" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
+    </row>
+    <row r="42" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+    </row>
+    <row r="43" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="20"/>
+      <c r="M43" s="20"/>
+    </row>
+    <row r="44" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
+    </row>
+    <row r="45" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="19"/>
+      <c r="M45" s="19"/>
+    </row>
+    <row r="46" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="19"/>
+      <c r="L46" s="19"/>
+      <c r="M46" s="19"/>
+    </row>
+    <row r="47" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="19"/>
+      <c r="L47" s="19"/>
+      <c r="M47" s="19"/>
+    </row>
+    <row r="48" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19"/>
+      <c r="K48" s="19"/>
+      <c r="L48" s="19"/>
+      <c r="M48" s="19"/>
+    </row>
+    <row r="49" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
+      <c r="J49" s="19"/>
+      <c r="K49" s="19"/>
+      <c r="L49" s="19"/>
+      <c r="M49" s="19"/>
+    </row>
+    <row r="50" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="19"/>
+    </row>
+    <row r="51" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="19"/>
+      <c r="M51" s="19"/>
+    </row>
+    <row r="52" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="20"/>
+      <c r="L52" s="20"/>
+      <c r="M52" s="20"/>
+    </row>
+    <row r="53" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
+      <c r="J53" s="19"/>
+      <c r="K53" s="19"/>
+      <c r="L53" s="19"/>
+      <c r="M53" s="19"/>
+    </row>
+    <row r="54" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="19"/>
+      <c r="K54" s="19"/>
+      <c r="L54" s="19"/>
+      <c r="M54" s="19"/>
+    </row>
+    <row r="55" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="19"/>
+      <c r="K55" s="19"/>
+      <c r="L55" s="19"/>
+      <c r="M55" s="19"/>
+    </row>
+    <row r="56" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="19"/>
+      <c r="K56" s="19"/>
+      <c r="L56" s="19"/>
+      <c r="M56" s="19"/>
+    </row>
+    <row r="57" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="19"/>
+      <c r="K57" s="19"/>
+      <c r="L57" s="19"/>
+      <c r="M57" s="19"/>
+    </row>
+    <row r="58" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H58" s="19"/>
+      <c r="I58" s="19"/>
+      <c r="J58" s="19"/>
+      <c r="K58" s="19"/>
+      <c r="L58" s="19"/>
+      <c r="M58" s="19"/>
+    </row>
+    <row r="59" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="19"/>
+      <c r="K59" s="19"/>
+      <c r="L59" s="19"/>
+      <c r="M59" s="19"/>
+    </row>
+    <row r="60" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H60" s="19"/>
+      <c r="I60" s="19"/>
+      <c r="J60" s="19"/>
+      <c r="K60" s="19"/>
+      <c r="L60" s="19"/>
+      <c r="M60" s="19"/>
+    </row>
+    <row r="61" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
+      <c r="J61" s="20"/>
+      <c r="K61" s="20"/>
+      <c r="L61" s="20"/>
+      <c r="M61" s="20"/>
+    </row>
+    <row r="62" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H62" s="19"/>
+      <c r="I62" s="19"/>
+      <c r="J62" s="19"/>
+      <c r="K62" s="19"/>
+      <c r="L62" s="19"/>
+      <c r="M62" s="19"/>
+    </row>
+    <row r="63" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="19"/>
+      <c r="K63" s="19"/>
+      <c r="L63" s="19"/>
+      <c r="M63" s="19"/>
+    </row>
+    <row r="64" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H64" s="19"/>
+      <c r="I64" s="19"/>
+      <c r="J64" s="19"/>
+      <c r="K64" s="19"/>
+      <c r="L64" s="19"/>
+      <c r="M64" s="19"/>
+    </row>
+    <row r="65" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H65" s="19"/>
+      <c r="I65" s="19"/>
+      <c r="J65" s="19"/>
+      <c r="K65" s="19"/>
+      <c r="L65" s="19"/>
+      <c r="M65" s="19"/>
+    </row>
+    <row r="66" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H66" s="19"/>
+      <c r="I66" s="19"/>
+      <c r="J66" s="19"/>
+      <c r="K66" s="19"/>
+      <c r="L66" s="19"/>
+      <c r="M66" s="19"/>
+    </row>
+    <row r="67" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H67" s="19"/>
+      <c r="I67" s="19"/>
+      <c r="J67" s="19"/>
+      <c r="K67" s="19"/>
+      <c r="L67" s="19"/>
+      <c r="M67" s="19"/>
+    </row>
+    <row r="68" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H68" s="19"/>
+      <c r="I68" s="19"/>
+      <c r="J68" s="19"/>
+      <c r="K68" s="19"/>
+      <c r="L68" s="19"/>
+      <c r="M68" s="19"/>
+    </row>
+    <row r="69" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H69" s="20"/>
+      <c r="I69" s="20"/>
+      <c r="J69" s="20"/>
+      <c r="K69" s="20"/>
+      <c r="L69" s="20"/>
+      <c r="M69" s="20"/>
+    </row>
+    <row r="70" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H70" s="20"/>
+      <c r="I70" s="20"/>
+      <c r="J70" s="20"/>
+      <c r="K70" s="20"/>
+      <c r="L70" s="20"/>
+      <c r="M70" s="20"/>
+    </row>
+    <row r="71" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H71" s="19"/>
+      <c r="I71" s="19"/>
+      <c r="J71" s="19"/>
+      <c r="K71" s="19"/>
+      <c r="L71" s="19"/>
+      <c r="M71" s="19"/>
+    </row>
+    <row r="72" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H72" s="19"/>
+      <c r="I72" s="19"/>
+      <c r="J72" s="19"/>
+      <c r="K72" s="19"/>
+      <c r="L72" s="19"/>
+      <c r="M72" s="19"/>
+    </row>
+    <row r="73" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H73" s="19"/>
+      <c r="I73" s="19"/>
+      <c r="J73" s="19"/>
+      <c r="K73" s="19"/>
+      <c r="L73" s="19"/>
+      <c r="M73" s="19"/>
+    </row>
+    <row r="74" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H74" s="19"/>
+      <c r="I74" s="19"/>
+      <c r="J74" s="19"/>
+      <c r="K74" s="19"/>
+      <c r="L74" s="19"/>
+      <c r="M74" s="19"/>
+    </row>
+    <row r="75" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H75" s="19"/>
+      <c r="I75" s="19"/>
+      <c r="J75" s="19"/>
+      <c r="K75" s="19"/>
+      <c r="L75" s="19"/>
+      <c r="M75" s="19"/>
+    </row>
+    <row r="76" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H76" s="19"/>
+      <c r="I76" s="19"/>
+      <c r="J76" s="19"/>
+      <c r="K76" s="19"/>
+      <c r="L76" s="19"/>
+      <c r="M76" s="19"/>
+    </row>
+    <row r="77" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H77" s="19"/>
+      <c r="I77" s="19"/>
+      <c r="J77" s="19"/>
+      <c r="K77" s="19"/>
+      <c r="L77" s="19"/>
+      <c r="M77" s="19"/>
+    </row>
+    <row r="78" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H78" s="19"/>
+      <c r="I78" s="19"/>
+      <c r="J78" s="19"/>
+      <c r="K78" s="19"/>
+      <c r="L78" s="19"/>
+      <c r="M78" s="19"/>
+    </row>
+    <row r="79" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H79" s="20"/>
+      <c r="I79" s="20"/>
+      <c r="J79" s="20"/>
+      <c r="K79" s="20"/>
+      <c r="L79" s="20"/>
+      <c r="M79" s="20"/>
+    </row>
+    <row r="80" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H80" s="20"/>
+      <c r="I80" s="20"/>
+      <c r="J80" s="20"/>
+      <c r="K80" s="20"/>
+      <c r="L80" s="20"/>
+      <c r="M80" s="20"/>
+    </row>
+    <row r="81" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H81" s="20"/>
+      <c r="I81" s="20"/>
+      <c r="J81" s="20"/>
+      <c r="K81" s="20"/>
+      <c r="L81" s="20"/>
+      <c r="M81" s="20"/>
+    </row>
+    <row r="82" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H82" s="24"/>
+      <c r="I82" s="24"/>
+      <c r="J82" s="24"/>
+      <c r="K82" s="24"/>
+      <c r="L82" s="24"/>
+      <c r="M82" s="24"/>
+    </row>
+    <row r="83" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H83" s="24"/>
+      <c r="I83" s="24"/>
+      <c r="J83" s="24"/>
+      <c r="K83" s="24"/>
+      <c r="L83" s="24"/>
+      <c r="M83" s="24"/>
+    </row>
+    <row r="84" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H84" s="24"/>
+      <c r="I84" s="24"/>
+      <c r="J84" s="24"/>
+      <c r="K84" s="24"/>
+      <c r="L84" s="24"/>
+      <c r="M84" s="24"/>
+    </row>
+    <row r="85" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H85" s="24"/>
+      <c r="I85" s="24"/>
+      <c r="J85" s="24"/>
+      <c r="K85" s="24"/>
+      <c r="L85" s="24"/>
+      <c r="M85" s="24"/>
+    </row>
+    <row r="86" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H86" s="24"/>
+      <c r="I86" s="24"/>
+      <c r="J86" s="24"/>
+      <c r="K86" s="24"/>
+      <c r="L86" s="24"/>
+      <c r="M86" s="24"/>
+    </row>
+    <row r="87" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H87" s="24"/>
+      <c r="I87" s="24"/>
+      <c r="J87" s="24"/>
+      <c r="K87" s="24"/>
+      <c r="L87" s="24"/>
+      <c r="M87" s="24"/>
+    </row>
+    <row r="88" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H88" s="24"/>
+      <c r="I88" s="24"/>
+      <c r="J88" s="24"/>
+      <c r="K88" s="24"/>
+      <c r="L88" s="24"/>
+      <c r="M88" s="24"/>
+    </row>
+    <row r="89" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H89" s="24"/>
+      <c r="I89" s="24"/>
+      <c r="J89" s="24"/>
+      <c r="K89" s="24"/>
+      <c r="L89" s="24"/>
+      <c r="M89" s="24"/>
+    </row>
+    <row r="90" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H90" s="24"/>
+      <c r="I90" s="24"/>
+      <c r="J90" s="24"/>
+      <c r="K90" s="24"/>
+      <c r="L90" s="24"/>
+      <c r="M90" s="24"/>
+    </row>
+    <row r="91" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H91" s="24"/>
+      <c r="I91" s="24"/>
+      <c r="J91" s="24"/>
+      <c r="K91" s="24"/>
+      <c r="L91" s="24"/>
+      <c r="M91" s="24"/>
+    </row>
+    <row r="92" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H92" s="24"/>
+      <c r="I92" s="24"/>
+      <c r="J92" s="24"/>
+      <c r="K92" s="24"/>
+      <c r="L92" s="24"/>
+      <c r="M92" s="24"/>
+    </row>
+    <row r="93" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H93" s="20"/>
+      <c r="I93" s="20"/>
+      <c r="J93" s="20"/>
+      <c r="K93" s="20"/>
+      <c r="L93" s="20"/>
+      <c r="M93" s="20"/>
+    </row>
+    <row r="94" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H94" s="20"/>
+      <c r="I94" s="20"/>
+      <c r="J94" s="20"/>
+      <c r="K94" s="20"/>
+      <c r="L94" s="20"/>
+      <c r="M94" s="20"/>
+    </row>
+    <row r="95" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H95" s="20"/>
+      <c r="I95" s="20"/>
+      <c r="J95" s="20"/>
+      <c r="K95" s="20"/>
+      <c r="L95" s="20"/>
+      <c r="M95" s="20"/>
+    </row>
+    <row r="96" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H96" s="20"/>
+      <c r="I96" s="20"/>
+      <c r="J96" s="20"/>
+      <c r="K96" s="20"/>
+      <c r="L96" s="20"/>
+      <c r="M96" s="20"/>
+    </row>
+    <row r="97" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H97" s="20"/>
+      <c r="I97" s="20"/>
+      <c r="J97" s="20"/>
+      <c r="K97" s="20"/>
+      <c r="L97" s="20"/>
+      <c r="M97" s="20"/>
+    </row>
+    <row r="98" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H98" s="20"/>
+      <c r="I98" s="20"/>
+      <c r="J98" s="20"/>
+      <c r="K98" s="20"/>
+      <c r="L98" s="20"/>
+      <c r="M98" s="20"/>
+    </row>
+    <row r="99" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H99" s="20"/>
+      <c r="I99" s="20"/>
+      <c r="J99" s="20"/>
+      <c r="K99" s="20"/>
+      <c r="L99" s="20"/>
+      <c r="M99" s="20"/>
+    </row>
+    <row r="100" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H100" s="20"/>
+      <c r="I100" s="20"/>
+      <c r="J100" s="20"/>
+      <c r="K100" s="20"/>
+      <c r="L100" s="20"/>
+      <c r="M100" s="20"/>
+    </row>
+    <row r="101" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H101" s="20"/>
+      <c r="I101" s="20"/>
+      <c r="J101" s="20"/>
+      <c r="K101" s="20"/>
+      <c r="L101" s="20"/>
+      <c r="M101" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1906,270 +2445,270 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="4" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
     </row>
     <row r="6" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="20"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>